<commit_message>
finally the end, thank you everyone
</commit_message>
<xml_diff>
--- a/public/help.xlsx
+++ b/public/help.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murrutiam\Desktop\apk\indicadores\dash-ariztia\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61A7F2A-14DB-40E6-9212-6EFA33BB789E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24C3551-2283-4182-BB19-4DD28EB19D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="501" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="501" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gant Proyect" sheetId="7" r:id="rId1"/>
@@ -832,9 +832,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79E930C-253D-491D-94C6-681541A17DDB}">
   <dimension ref="A1:AE63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,11 +1256,21 @@
       <c r="P10" s="8"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
+      <c r="S10" s="23">
+        <v>13</v>
+      </c>
+      <c r="T10" s="23">
+        <v>14</v>
+      </c>
+      <c r="U10" s="23">
+        <v>15</v>
+      </c>
+      <c r="V10" s="23">
+        <v>16</v>
+      </c>
+      <c r="W10" s="23">
+        <v>17</v>
+      </c>
       <c r="X10" s="7"/>
       <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
@@ -2609,8 +2619,12 @@
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="24"/>
-      <c r="O48" s="24"/>
-      <c r="P48" s="24"/>
+      <c r="O48" s="24">
+        <v>7</v>
+      </c>
+      <c r="P48" s="24">
+        <v>8</v>
+      </c>
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
       <c r="S48" s="4"/>
@@ -2644,8 +2658,12 @@
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="24"/>
-      <c r="O49" s="24"/>
-      <c r="P49" s="24"/>
+      <c r="O49" s="24">
+        <v>7</v>
+      </c>
+      <c r="P49" s="24">
+        <v>8</v>
+      </c>
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
       <c r="S49" s="4"/>
@@ -2680,7 +2698,9 @@
       <c r="M50" s="2"/>
       <c r="N50" s="24"/>
       <c r="O50" s="24"/>
-      <c r="P50" s="24"/>
+      <c r="P50" s="24">
+        <v>9</v>
+      </c>
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
       <c r="S50" s="4"/>
@@ -2751,7 +2771,9 @@
       <c r="N53" s="10"/>
       <c r="O53" s="10"/>
       <c r="P53" s="10"/>
-      <c r="Q53" s="28"/>
+      <c r="Q53" s="28">
+        <v>10</v>
+      </c>
       <c r="R53" s="9"/>
       <c r="S53" s="9"/>
       <c r="T53" s="9"/>
@@ -2786,7 +2808,9 @@
       <c r="N54" s="8"/>
       <c r="O54" s="8"/>
       <c r="P54" s="8"/>
-      <c r="Q54" s="23"/>
+      <c r="Q54" s="23">
+        <v>10</v>
+      </c>
       <c r="R54" s="7"/>
       <c r="S54" s="7"/>
       <c r="T54" s="7"/>
@@ -2857,7 +2881,9 @@
       <c r="O56" s="10"/>
       <c r="P56" s="10"/>
       <c r="Q56" s="9"/>
-      <c r="R56" s="28"/>
+      <c r="R56" s="28">
+        <v>11</v>
+      </c>
       <c r="S56" s="9"/>
       <c r="T56" s="9"/>
       <c r="U56" s="9"/>
@@ -2892,7 +2918,9 @@
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
       <c r="Q57" s="4"/>
-      <c r="R57" s="20"/>
+      <c r="R57" s="20">
+        <v>12</v>
+      </c>
       <c r="S57" s="4"/>
       <c r="T57" s="4"/>
       <c r="U57" s="4"/>
@@ -3057,8 +3085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4214072A-4089-4AB3-A96D-300F5C38EAA9}">
   <dimension ref="A1:AF63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>